<commit_message>
AIC Table Fix 2
</commit_message>
<xml_diff>
--- a/Tables/region_deltaAIC.xlsx
+++ b/Tables/region_deltaAIC.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a Papers/Rapid_drought/Paper 3/climate_lag/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6B9AD2-D988-F949-A861-CC77155925D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB4A020-3767-6D4F-8A8F-88108582A555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="29160" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="north_deltaAIC" sheetId="1" r:id="rId1"/>
+    <sheet name="Old" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="15">
   <si>
     <t>SLA</t>
   </si>
@@ -66,15 +67,12 @@
   <si>
     <t>Old</t>
   </si>
-  <si>
-    <t>New</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,8 +207,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +407,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -575,19 +594,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -600,13 +613,25 @@
     <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -964,67 +989,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I16" sqref="A14:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="12"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1050,109 +1047,57 @@
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>3.7336520336111798</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>5.4286078623426901</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>6.59687212451718</v>
       </c>
       <c r="F5" s="3">
         <v>0.839153787816031</v>
       </c>
-      <c r="G5" s="4">
-        <v>4.79937942817378</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="5">
+        <v>3.8109627725098099</v>
+      </c>
+      <c r="H5" s="5">
         <v>3.8001214167361499</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>4.7326876455863403</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="11">
-        <v>0</v>
-      </c>
-      <c r="M5" s="10">
-        <v>3.7336520336111798</v>
-      </c>
-      <c r="N5" s="10">
-        <v>3.8001214167361499</v>
-      </c>
-      <c r="O5" s="10">
-        <v>4.7326876455863403</v>
-      </c>
-      <c r="P5" s="11">
-        <v>0.839153787816031</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>3.8109627725098099</v>
-      </c>
-      <c r="R5" s="10">
-        <v>5.4286078623426901</v>
-      </c>
-      <c r="S5" s="10">
-        <v>6.59687212451718</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>4.4871670892916899</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>3.10024836442062</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>2.9094722636982602</v>
       </c>
       <c r="G6" s="3">
-        <v>0.98841665566396797</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
         <v>1.5211760539496</v>
@@ -1160,55 +1105,28 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="10">
-        <v>4.4871670892916899</v>
-      </c>
-      <c r="M6" s="11">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11">
-        <v>1.5211760539496</v>
-      </c>
-      <c r="O6" s="11">
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
-        <v>2.9094722636982602</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>0</v>
-      </c>
-      <c r="R6" s="10">
-        <v>3.10024836442062</v>
-      </c>
-      <c r="S6" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>2.6639739267811802</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>5.2851720342341704</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>3.0631253632209301</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="4">
-        <v>3.9942140167177098</v>
+      <c r="G7" s="5">
+        <v>3.0057973610537401</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -1216,191 +1134,90 @@
       <c r="I7" s="3">
         <v>1.5884064427646101</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="10">
-        <v>2.6639739267811802</v>
-      </c>
-      <c r="M7" s="10">
-        <v>5.2851720342341704</v>
-      </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
-      <c r="O7" s="11">
-        <v>1.5884064427646101</v>
-      </c>
-      <c r="P7" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10">
-        <v>3.0057973610537401</v>
-      </c>
-      <c r="R7" s="11">
-        <v>0</v>
-      </c>
-      <c r="S7" s="10">
-        <v>3.0631253632209301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>5.54277116833146</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>5.6667271909109296</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>8.2552909737169102</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>10.346263610713301</v>
       </c>
-      <c r="F8" s="4">
-        <v>2.89062889340858</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.277703862165254</v>
-      </c>
-      <c r="H8" s="4">
-        <v>3.1911807252708999</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3.4385289062347502</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="10">
-        <v>5.54277116833146</v>
-      </c>
-      <c r="M8" s="10">
-        <v>5.6667271909109296</v>
-      </c>
-      <c r="N8" s="10">
+      <c r="F8" s="5">
+        <v>5.6632176169532604</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2.0618761736432099</v>
+      </c>
+      <c r="H8" s="5">
         <v>5.9637694475113703</v>
       </c>
-      <c r="O8" s="10">
+      <c r="I8" s="5">
         <v>6.2111173256507799</v>
       </c>
-      <c r="P8" s="10">
-        <v>5.6632176169532604</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>2.0618761736432099</v>
-      </c>
-      <c r="R8" s="10">
-        <v>8.2552909737169102</v>
-      </c>
-      <c r="S8" s="10">
-        <v>10.346263610713301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>6.7504560562010703</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>6.77865668647883</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>9.5578848922796205</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>9.9839878375360094</v>
       </c>
-      <c r="F9" s="2">
-        <v>1.329808501554</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>2.8183558662785799</v>
-      </c>
-      <c r="I9" s="5">
-        <v>3.3072114354763502</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="10">
-        <v>6.7504560562010703</v>
-      </c>
-      <c r="M9" s="10">
-        <v>6.77865668647883</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="F9" s="6">
+        <v>5.72425767277673</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3.406032497659</v>
+      </c>
+      <c r="H9" s="6">
         <v>7.2128050376213704</v>
       </c>
-      <c r="O9" s="10">
+      <c r="I9" s="6">
         <v>7.7016605643293596</v>
       </c>
-      <c r="P9" s="10">
-        <v>5.72425767277673</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>3.406032497659</v>
-      </c>
-      <c r="R9" s="10">
-        <v>9.5578848922796205</v>
-      </c>
-      <c r="S9" s="10">
-        <v>9.9839878375360094</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="S12" s="12"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1426,33 +1243,8 @@
       <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1468,47 +1260,20 @@
       <c r="E14" s="3">
         <v>1.1816999528337</v>
       </c>
-      <c r="F14" s="7">
-        <v>2.5356571564934698</v>
+      <c r="F14" s="3">
+        <v>2.0047315682331801</v>
       </c>
       <c r="G14" s="3">
-        <v>1.3220345833024101</v>
+        <v>1.07967903313238</v>
       </c>
       <c r="H14" s="3">
         <v>1.4360697785487</v>
       </c>
       <c r="I14" s="3">
-        <v>1.6378161809379901</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="11">
-        <v>1.8133356846028601</v>
-      </c>
-      <c r="M14" s="11">
-        <v>0.27318532657318401</v>
-      </c>
-      <c r="N14" s="11">
-        <v>1.4360697785487</v>
-      </c>
-      <c r="O14" s="11">
-        <v>1.6378161809379901</v>
-      </c>
-      <c r="P14" s="10">
-        <v>2.0047315236097298</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>1.07967903313238</v>
-      </c>
-      <c r="R14" s="11">
-        <v>0.15587050898466301</v>
-      </c>
-      <c r="S14" s="11">
-        <v>1.1816999528337</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1.63778673820798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1525,10 +1290,10 @@
         <v>0.82199319205574295</v>
       </c>
       <c r="F15" s="3">
-        <v>0.53092558826028802</v>
-      </c>
-      <c r="G15" s="7">
-        <v>2.4839716718333902</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2.2416161216633599</v>
       </c>
       <c r="H15" s="3">
         <v>0</v>
@@ -1536,35 +1301,8 @@
       <c r="I15" s="3">
         <v>1.6535418950688801</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="11">
-        <v>0.73366976001125295</v>
-      </c>
-      <c r="M15" s="11">
-        <v>1.9936502075679501</v>
-      </c>
-      <c r="N15" s="11">
-        <v>0</v>
-      </c>
-      <c r="O15" s="11">
-        <v>1.6535418950688801</v>
-      </c>
-      <c r="P15" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>2.2416161216633599</v>
-      </c>
-      <c r="R15" s="11">
-        <v>1.2993382831809901</v>
-      </c>
-      <c r="S15" s="11">
-        <v>0.82199319205574295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -1581,10 +1319,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>1.9689032710157299</v>
+        <v>1.43797768275545</v>
       </c>
       <c r="G16" s="3">
-        <v>0.24235555017003199</v>
+        <v>0</v>
       </c>
       <c r="H16" s="3">
         <v>0.66997765813903198</v>
@@ -1592,191 +1330,90 @@
       <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="11">
-        <v>0</v>
-      </c>
-      <c r="M16" s="11">
-        <v>0</v>
-      </c>
-      <c r="N16" s="11">
-        <v>0.66997765813903198</v>
-      </c>
-      <c r="O16" s="11">
-        <v>0</v>
-      </c>
-      <c r="P16" s="11">
-        <v>1.43797768275545</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>0</v>
-      </c>
-      <c r="R16" s="11">
-        <v>0</v>
-      </c>
-      <c r="S16" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>3.5313665424691898</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>3.0519147807326599</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>2.7574228711218902</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>3.11952141237634</v>
       </c>
-      <c r="F17" s="7">
-        <v>2.3057685799103602</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.51314585123873302</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0.41058154850543399</v>
-      </c>
-      <c r="I17" s="3">
-        <v>1.7930955581632599</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="10">
-        <v>3.5313665424691898</v>
-      </c>
-      <c r="M17" s="10">
-        <v>3.0519147807326599</v>
-      </c>
-      <c r="N17" s="10">
+      <c r="F17" s="5">
+        <v>4.5474316785730498</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3.0433790271736099</v>
+      </c>
+      <c r="H17" s="5">
         <v>3.1831698052847099</v>
       </c>
-      <c r="O17" s="10">
+      <c r="I17" s="5">
         <v>4.5656842801181501</v>
       </c>
-      <c r="P17" s="10">
-        <v>4.5474316785730498</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>3.0433790271736099</v>
-      </c>
-      <c r="R17" s="10">
-        <v>2.7574228711218902</v>
-      </c>
-      <c r="S17" s="10">
-        <v>3.11952141237634</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>2.3537068694240602</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="6">
         <v>4.2580934741317797</v>
       </c>
       <c r="D18" s="2">
         <v>1.85291601837162</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="6">
         <v>4.7696634953354096</v>
       </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.18209847578327801</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1.33284051786723</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L18" s="10">
-        <v>2.3537068694240602</v>
-      </c>
-      <c r="M18" s="10">
-        <v>4.2580934741317797</v>
-      </c>
-      <c r="N18" s="10">
+      <c r="F18" s="6">
+        <v>3.8635237908529199</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4.15209360308745</v>
+      </c>
+      <c r="H18" s="6">
         <v>4.5765476313008504</v>
       </c>
-      <c r="O18" s="10">
+      <c r="I18" s="6">
         <v>5.72728967433068</v>
       </c>
-      <c r="P18" s="10">
-        <v>3.8635237908529199</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>4.15209360308745</v>
-      </c>
-      <c r="R18" s="11">
-        <v>1.85291601837162</v>
-      </c>
-      <c r="S18" s="10">
-        <v>4.7696634953354096</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="S21" s="12"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>0</v>
@@ -1802,33 +1439,8 @@
       <c r="I22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -1844,51 +1456,24 @@
       <c r="E23" s="3">
         <v>0</v>
       </c>
-      <c r="F23" s="7">
-        <v>4.6174531374726904</v>
-      </c>
-      <c r="G23" s="7">
-        <v>4.4037305099536797</v>
+      <c r="F23" s="3">
+        <v>0.22300399140749499</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.4747420319972702</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="5">
         <v>4.3257076065001501</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L23" s="11">
-        <v>0</v>
-      </c>
-      <c r="M23" s="11">
-        <v>1.0838742471987599</v>
-      </c>
-      <c r="N23" s="11">
-        <v>0</v>
-      </c>
-      <c r="O23" s="10">
-        <v>4.3257076065001501</v>
-      </c>
-      <c r="P23" s="11">
-        <v>0.22300399140749499</v>
-      </c>
-      <c r="Q23" s="10">
-        <v>2.4747420319972702</v>
-      </c>
-      <c r="R23" s="11">
-        <v>0</v>
-      </c>
-      <c r="S23" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>2.5556960086787499</v>
       </c>
       <c r="C24" s="3">
@@ -1900,169 +1485,88 @@
       <c r="E24" s="3">
         <v>0.456913491571868</v>
       </c>
-      <c r="F24" s="7">
-        <v>4.9724472388488703</v>
-      </c>
-      <c r="G24" s="7">
-        <v>4.0753628230895602</v>
-      </c>
-      <c r="H24" s="7">
+      <c r="F24" s="3">
+        <v>0.57799809278367298</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2.1463743451331498</v>
+      </c>
+      <c r="H24" s="5">
         <v>8.5773135244990009</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="5">
         <v>3.8220469945590598</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L24" s="10">
-        <v>2.5556960086787499</v>
-      </c>
-      <c r="M24" s="11">
-        <v>0.76052608427016799</v>
-      </c>
-      <c r="N24" s="10">
-        <v>8.5773135244990009</v>
-      </c>
-      <c r="O24" s="10">
-        <v>3.8220469945590598</v>
-      </c>
-      <c r="P24" s="11">
-        <v>0.57799809278367298</v>
-      </c>
-      <c r="Q24" s="10">
-        <v>2.1463743451331498</v>
-      </c>
-      <c r="R24" s="11">
-        <v>0.75504115223247903</v>
-      </c>
-      <c r="S24" s="11">
-        <v>0.456913491571868</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>2.9619386356353101</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>3.39141759535869</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>2.4798191604149902</v>
       </c>
-      <c r="F25" s="7">
-        <v>6.1671321743706402</v>
+      <c r="F25" s="3">
+        <v>1.77268302830544</v>
       </c>
       <c r="G25" s="3">
-        <v>1.9289884779564099</v>
-      </c>
-      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
         <v>9.0685485284275291</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="10">
-        <v>2.9619386356353101</v>
-      </c>
-      <c r="M25" s="11">
-        <v>0</v>
-      </c>
-      <c r="N25" s="10">
-        <v>9.0685485284275291</v>
-      </c>
-      <c r="O25" s="11">
-        <v>0</v>
-      </c>
-      <c r="P25" s="11">
-        <v>1.77268302830544</v>
-      </c>
-      <c r="Q25" s="11">
-        <v>0</v>
-      </c>
-      <c r="R25" s="10">
-        <v>3.39141759535869</v>
-      </c>
-      <c r="S25" s="10">
-        <v>2.4798191604149902</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>2.73008643232424</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>3.42765313245854</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>2.3924235224567401</v>
       </c>
       <c r="E26" s="3">
         <v>0.60246024539082998</v>
       </c>
-      <c r="F26" s="7">
-        <v>2.82987414373292</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3.0320249053920598</v>
-      </c>
-      <c r="H26" s="7">
-        <v>3.5301393896088502</v>
-      </c>
-      <c r="I26" s="7">
-        <v>4.0299997336360303</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="10">
-        <v>2.73008643232424</v>
-      </c>
-      <c r="M26" s="10">
-        <v>3.42765313245854</v>
-      </c>
-      <c r="N26" s="10">
+      <c r="F26" s="3">
+        <v>1.2080137205093699</v>
+      </c>
+      <c r="G26" s="5">
+        <v>3.8756251323893598</v>
+      </c>
+      <c r="H26" s="5">
         <v>6.3027281117883804</v>
       </c>
-      <c r="O26" s="10">
+      <c r="I26" s="5">
         <v>6.8025884987146101</v>
       </c>
-      <c r="P26" s="11">
-        <v>1.2080137205093699</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>3.8756251323893598</v>
-      </c>
-      <c r="R26" s="10">
-        <v>2.3924235224567401</v>
-      </c>
-      <c r="S26" s="11">
-        <v>0.60246024539082998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>1.1860743348443099</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <v>3.8589530061244699</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <v>3.5982127671813902</v>
       </c>
       <c r="E27" s="2">
@@ -2071,69 +1575,706 @@
       <c r="F27" s="2">
         <v>0</v>
       </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="8">
-        <v>3.86713240648987</v>
-      </c>
-      <c r="I27" s="8">
-        <v>2.9595458616049699</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="G27" s="6">
+        <v>2.4654606688000098</v>
+      </c>
+      <c r="H27" s="6">
+        <v>8.2615815611625294</v>
+      </c>
+      <c r="I27" s="6">
+        <v>7.3539950432350496</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1023BD-F139-A542-9ACE-3FDF8CD95FA1}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3.73</v>
+      </c>
+      <c r="D5" s="14">
+        <v>5.43</v>
+      </c>
+      <c r="E5" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.84</v>
+      </c>
+      <c r="G5" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="H5" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="I5" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4.49</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2.91</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1.52</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.66</v>
+      </c>
+      <c r="C7" s="14">
+        <v>5.29</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>3.06</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14">
+        <v>5.54</v>
+      </c>
+      <c r="C8" s="14">
+        <v>5.67</v>
+      </c>
+      <c r="D8" s="14">
+        <v>8.26</v>
+      </c>
+      <c r="E8" s="14">
+        <v>10.35</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2.89</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H8" s="14">
+        <v>3.19</v>
+      </c>
+      <c r="I8" s="14">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L27" s="11">
-        <v>1.1860743348443099</v>
-      </c>
-      <c r="M27" s="10">
-        <v>3.8589530061244699</v>
-      </c>
-      <c r="N27" s="10">
-        <v>8.2615815611625294</v>
-      </c>
-      <c r="O27" s="10">
-        <v>7.3539950432350496</v>
-      </c>
-      <c r="P27" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
-        <v>2.4654606688000098</v>
-      </c>
-      <c r="R27" s="10">
-        <v>3.5982127671813902</v>
-      </c>
-      <c r="S27" s="11">
-        <v>1.2449146520066301</v>
+      <c r="B9" s="15">
+        <v>6.75</v>
+      </c>
+      <c r="C9" s="15">
+        <v>6.78</v>
+      </c>
+      <c r="D9" s="15">
+        <v>9.56</v>
+      </c>
+      <c r="E9" s="15">
+        <v>9.98</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1.33</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2.82</v>
+      </c>
+      <c r="I9" s="15">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1.81</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.27</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1.18</v>
+      </c>
+      <c r="F14" s="14">
+        <v>2.54</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1.32</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1.44</v>
+      </c>
+      <c r="I14" s="13">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1.99</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.82</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0.53</v>
+      </c>
+      <c r="G15" s="14">
+        <v>2.48</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1.97</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.24</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0.67</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="14">
+        <v>3.53</v>
+      </c>
+      <c r="C17" s="14">
+        <v>3.05</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2.76</v>
+      </c>
+      <c r="E17" s="14">
+        <v>3.12</v>
+      </c>
+      <c r="F17" s="14">
+        <v>2.31</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.51</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0.41</v>
+      </c>
+      <c r="I17" s="13">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2.35</v>
+      </c>
+      <c r="C18" s="15">
+        <v>4.26</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1.85</v>
+      </c>
+      <c r="E18" s="15">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13">
+        <v>0</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1.08</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="14">
+        <v>4.62</v>
+      </c>
+      <c r="G23" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="14">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="14">
+        <v>2.56</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.46</v>
+      </c>
+      <c r="F24" s="14">
+        <v>4.97</v>
+      </c>
+      <c r="G24" s="14">
+        <v>4.08</v>
+      </c>
+      <c r="H24" s="14">
+        <v>8.58</v>
+      </c>
+      <c r="I24" s="14">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="14">
+        <v>2.96</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0</v>
+      </c>
+      <c r="D25" s="14">
+        <v>3.39</v>
+      </c>
+      <c r="E25" s="14">
+        <v>2.48</v>
+      </c>
+      <c r="F25" s="14">
+        <v>6.17</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1.93</v>
+      </c>
+      <c r="H25" s="14">
+        <v>9.07</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="14">
+        <v>2.73</v>
+      </c>
+      <c r="C26" s="14">
+        <v>3.43</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2.39</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="F26" s="14">
+        <v>2.83</v>
+      </c>
+      <c r="G26" s="14">
+        <v>3.03</v>
+      </c>
+      <c r="H26" s="14">
+        <v>3.53</v>
+      </c>
+      <c r="I26" s="14">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1.19</v>
+      </c>
+      <c r="C27" s="15">
+        <v>3.86</v>
+      </c>
+      <c r="D27" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1.24</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="15">
+        <v>3.87</v>
+      </c>
+      <c r="I27" s="15">
+        <v>2.96</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="12">
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D21:E21"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R12:S12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>